<commit_message>
finished integration of pipes, updated some signals
</commit_message>
<xml_diff>
--- a/Project2/Lab Documents/Proj2_control_signals.xlsx
+++ b/Project2/Lab Documents/Proj2_control_signals.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="157">
   <si>
     <t xml:space="preserve">Datapath signals</t>
   </si>
@@ -451,9 +451,6 @@
     <t xml:space="preserve">w_PC_next</t>
   </si>
   <si>
-    <t xml:space="preserve">Maybe?</t>
-  </si>
-  <si>
     <t xml:space="preserve">w_MEM_PC_next</t>
   </si>
   <si>
@@ -467,6 +464,27 @@
   </si>
   <si>
     <t xml:space="preserve">w_WB_DMEM_out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s_DMEM_Lb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s_MEM_DMEM_Lb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s_WB_DMEM_Lb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s_DMEM_Lh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s_MEM_DMEM_Lh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s_WB_DMEM_Lh</t>
   </si>
   <si>
     <t xml:space="preserve">w_RegWrData</t>
@@ -506,7 +524,7 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -516,7 +534,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA6A6A6"/>
-        <bgColor rgb="FFA9D18E"/>
+        <bgColor rgb="FF999999"/>
       </patternFill>
     </fill>
     <fill>
@@ -528,7 +546,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF5B9BD5"/>
-        <bgColor rgb="FF808080"/>
+        <bgColor rgb="FF999999"/>
       </patternFill>
     </fill>
     <fill>
@@ -552,7 +570,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF548235"/>
-        <bgColor rgb="FF339966"/>
+        <bgColor rgb="FF808080"/>
       </patternFill>
     </fill>
     <fill>
@@ -570,7 +588,13 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF548235"/>
+        <bgColor rgb="FF999999"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF999999"/>
+        <bgColor rgb="FFA6A6A6"/>
       </patternFill>
     </fill>
   </fills>
@@ -615,7 +639,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -684,19 +708,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -785,7 +801,7 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFA9D18E"/>
       <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF5B9BD5"/>
+      <rgbColor rgb="FFA6A6A6"/>
       <rgbColor rgb="FFCC3399"/>
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFDAE3F3"/>
@@ -816,9 +832,9 @@
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF9966FF"/>
-      <rgbColor rgb="FFA6A6A6"/>
+      <rgbColor rgb="FF999999"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF5B9BD5"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
@@ -835,22 +851,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F34" activeCellId="0" sqref="F34"/>
+      <selection pane="topLeft" activeCell="D47" activeCellId="0" sqref="D47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="20.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="34.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="26.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="26.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1178,26 +1194,26 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" s="19" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="C16" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G16" s="18" t="s">
+      <c r="C16" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="11" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1245,133 +1261,133 @@
       </c>
       <c r="G18" s="11"/>
     </row>
-    <row r="19" s="19" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B19" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="17" t="s">
+      <c r="B19" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="D19" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G19" s="18"/>
-    </row>
-    <row r="20" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D19" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="11"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B20" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="17" t="s">
+      <c r="B20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D20" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G20" s="18"/>
-    </row>
-    <row r="21" s="19" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" s="11"/>
+    </row>
+    <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B21" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" s="17" t="s">
+      <c r="B21" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D21" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G21" s="18"/>
-    </row>
-    <row r="22" s="19" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D21" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="11"/>
+    </row>
+    <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B22" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="17" t="s">
+      <c r="B22" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D22" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G22" s="18"/>
-    </row>
-    <row r="23" s="19" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="18" t="s">
+      <c r="D22" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" s="11"/>
+    </row>
+    <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="B23" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" s="17" t="s">
+      <c r="B23" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="D23" s="17" t="s">
+      <c r="D23" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="E23" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G23" s="18" t="s">
+      <c r="E23" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" s="11" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="24" s="19" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="20" t="s">
+    <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="B24" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" s="17" t="s">
+      <c r="B24" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="D24" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G24" s="18"/>
+      <c r="D24" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" s="11"/>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="11" t="s">
@@ -1529,7 +1545,7 @@
       <c r="G31" s="11"/>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="20" t="s">
+      <c r="A32" s="17" t="s">
         <v>122</v>
       </c>
       <c r="B32" s="9" t="s">
@@ -1552,7 +1568,7 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="18" t="s">
+      <c r="A33" s="11" t="s">
         <v>125</v>
       </c>
       <c r="B33" s="9" t="s">
@@ -1573,7 +1589,7 @@
       <c r="G33" s="11"/>
     </row>
     <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="18" t="s">
+      <c r="A34" s="11" t="s">
         <v>129</v>
       </c>
       <c r="B34" s="9" t="s">
@@ -1594,7 +1610,7 @@
       <c r="G34" s="11"/>
     </row>
     <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="20" t="s">
+      <c r="A35" s="17" t="s">
         <v>132</v>
       </c>
       <c r="B35" s="9" t="s">
@@ -1617,7 +1633,7 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="20" t="s">
+      <c r="A36" s="17" t="s">
         <v>135</v>
       </c>
       <c r="B36" s="9" t="s">
@@ -1640,7 +1656,7 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="20" t="s">
+      <c r="A37" s="17" t="s">
         <v>138</v>
       </c>
       <c r="B37" s="9" t="s">
@@ -1661,7 +1677,7 @@
       <c r="G37" s="11"/>
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="20" t="s">
+      <c r="A38" s="17" t="s">
         <v>140</v>
       </c>
       <c r="B38" s="9" t="s">
@@ -1681,71 +1697,114 @@
       </c>
       <c r="G38" s="11"/>
     </row>
-    <row r="39" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="11" t="s">
+    <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="18" t="s">
         <v>142</v>
       </c>
       <c r="B39" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="C39" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" s="9" t="s">
+      <c r="F39" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" s="11" t="s">
         <v>144</v>
-      </c>
-      <c r="F39" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="G39" s="11" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="B40" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D40" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E40" s="9" t="s">
+      <c r="F40" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="F40" s="9" t="s">
+      <c r="G40" s="11"/>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="G40" s="11"/>
-    </row>
-    <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="11" t="s">
+      <c r="B41" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="9" t="s">
         <v>149</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>9</v>
       </c>
       <c r="F41" s="9" t="s">
         <v>150</v>
       </c>
       <c r="G41" s="11"/>
     </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="G42" s="11"/>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="G43" s="11"/>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
@@ -1774,7 +1833,7 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B37:F41">
+  <conditionalFormatting sqref="B37:F43">
     <cfRule type="cellIs" priority="8" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>"No"</formula>
     </cfRule>

</xml_diff>

<commit_message>
finished data avoidance for Bubblesort, still need to test both of them and...
</commit_message>
<xml_diff>
--- a/Project2/Lab Documents/Proj2_control_signals.xlsx
+++ b/Project2/Lab Documents/Proj2_control_signals.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="157">
   <si>
     <t xml:space="preserve">Datapath signals</t>
   </si>
@@ -451,9 +451,6 @@
     <t xml:space="preserve">w_PC_next</t>
   </si>
   <si>
-    <t xml:space="preserve">Maybe?</t>
-  </si>
-  <si>
     <t xml:space="preserve">w_MEM_PC_next</t>
   </si>
   <si>
@@ -467,6 +464,27 @@
   </si>
   <si>
     <t xml:space="preserve">w_WB_DMEM_out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s_DMEM_Lb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s_MEM_DMEM_Lb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s_WB_DMEM_Lb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s_DMEM_Lh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s_MEM_DMEM_Lh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s_WB_DMEM_Lh</t>
   </si>
   <si>
     <t xml:space="preserve">w_RegWrData</t>
@@ -506,7 +524,7 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -516,7 +534,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA6A6A6"/>
-        <bgColor rgb="FFA9D18E"/>
+        <bgColor rgb="FF999999"/>
       </patternFill>
     </fill>
     <fill>
@@ -528,7 +546,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF5B9BD5"/>
-        <bgColor rgb="FF808080"/>
+        <bgColor rgb="FF999999"/>
       </patternFill>
     </fill>
     <fill>
@@ -552,7 +570,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF548235"/>
-        <bgColor rgb="FF339966"/>
+        <bgColor rgb="FF808080"/>
       </patternFill>
     </fill>
     <fill>
@@ -570,7 +588,13 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF548235"/>
+        <bgColor rgb="FF999999"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF999999"/>
+        <bgColor rgb="FFA6A6A6"/>
       </patternFill>
     </fill>
   </fills>
@@ -615,7 +639,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -684,19 +708,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -785,7 +801,7 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFA9D18E"/>
       <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF5B9BD5"/>
+      <rgbColor rgb="FFA6A6A6"/>
       <rgbColor rgb="FFCC3399"/>
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFDAE3F3"/>
@@ -816,9 +832,9 @@
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF9966FF"/>
-      <rgbColor rgb="FFA6A6A6"/>
+      <rgbColor rgb="FF999999"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF5B9BD5"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
@@ -835,22 +851,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F34" activeCellId="0" sqref="F34"/>
+      <selection pane="topLeft" activeCell="D47" activeCellId="0" sqref="D47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="20.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="34.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="26.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="26.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1178,26 +1194,26 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" s="19" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="C16" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G16" s="18" t="s">
+      <c r="C16" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="11" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1245,133 +1261,133 @@
       </c>
       <c r="G18" s="11"/>
     </row>
-    <row r="19" s="19" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B19" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="17" t="s">
+      <c r="B19" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="D19" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G19" s="18"/>
-    </row>
-    <row r="20" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D19" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="11"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B20" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="17" t="s">
+      <c r="B20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D20" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G20" s="18"/>
-    </row>
-    <row r="21" s="19" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" s="11"/>
+    </row>
+    <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B21" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" s="17" t="s">
+      <c r="B21" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D21" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G21" s="18"/>
-    </row>
-    <row r="22" s="19" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D21" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="11"/>
+    </row>
+    <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B22" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="17" t="s">
+      <c r="B22" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D22" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G22" s="18"/>
-    </row>
-    <row r="23" s="19" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="18" t="s">
+      <c r="D22" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" s="11"/>
+    </row>
+    <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="B23" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" s="17" t="s">
+      <c r="B23" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="D23" s="17" t="s">
+      <c r="D23" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="E23" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G23" s="18" t="s">
+      <c r="E23" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" s="11" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="24" s="19" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="20" t="s">
+    <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="B24" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" s="17" t="s">
+      <c r="B24" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="D24" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G24" s="18"/>
+      <c r="D24" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" s="11"/>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="11" t="s">
@@ -1529,7 +1545,7 @@
       <c r="G31" s="11"/>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="20" t="s">
+      <c r="A32" s="17" t="s">
         <v>122</v>
       </c>
       <c r="B32" s="9" t="s">
@@ -1552,7 +1568,7 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="18" t="s">
+      <c r="A33" s="11" t="s">
         <v>125</v>
       </c>
       <c r="B33" s="9" t="s">
@@ -1573,7 +1589,7 @@
       <c r="G33" s="11"/>
     </row>
     <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="18" t="s">
+      <c r="A34" s="11" t="s">
         <v>129</v>
       </c>
       <c r="B34" s="9" t="s">
@@ -1594,7 +1610,7 @@
       <c r="G34" s="11"/>
     </row>
     <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="20" t="s">
+      <c r="A35" s="17" t="s">
         <v>132</v>
       </c>
       <c r="B35" s="9" t="s">
@@ -1617,7 +1633,7 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="20" t="s">
+      <c r="A36" s="17" t="s">
         <v>135</v>
       </c>
       <c r="B36" s="9" t="s">
@@ -1640,7 +1656,7 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="20" t="s">
+      <c r="A37" s="17" t="s">
         <v>138</v>
       </c>
       <c r="B37" s="9" t="s">
@@ -1661,7 +1677,7 @@
       <c r="G37" s="11"/>
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="20" t="s">
+      <c r="A38" s="17" t="s">
         <v>140</v>
       </c>
       <c r="B38" s="9" t="s">
@@ -1681,71 +1697,114 @@
       </c>
       <c r="G38" s="11"/>
     </row>
-    <row r="39" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="11" t="s">
+    <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="18" t="s">
         <v>142</v>
       </c>
       <c r="B39" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="C39" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" s="9" t="s">
+      <c r="F39" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" s="11" t="s">
         <v>144</v>
-      </c>
-      <c r="F39" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="G39" s="11" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="B40" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D40" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E40" s="9" t="s">
+      <c r="F40" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="F40" s="9" t="s">
+      <c r="G40" s="11"/>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="G40" s="11"/>
-    </row>
-    <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="11" t="s">
+      <c r="B41" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="9" t="s">
         <v>149</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>9</v>
       </c>
       <c r="F41" s="9" t="s">
         <v>150</v>
       </c>
       <c r="G41" s="11"/>
     </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="G42" s="11"/>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="G43" s="11"/>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
@@ -1774,7 +1833,7 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B37:F41">
+  <conditionalFormatting sqref="B37:F43">
     <cfRule type="cellIs" priority="8" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>"No"</formula>
     </cfRule>

</xml_diff>

<commit_message>
forgot to add the updated control signals
</commit_message>
<xml_diff>
--- a/Project2/Lab Documents/Proj2_control_signals.xlsx
+++ b/Project2/Lab Documents/Proj2_control_signals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\CPRE381\ProjectGit\cpre_381\Project2\Lab Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B630B74C-9C68-4158-95ED-BA56FEF4BA8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{505E2D6D-8336-4176-950D-91E835CD2C7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10005" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1144,7 +1144,7 @@
   <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>